<commit_message>
Updated requirements - Added album views
</commit_message>
<xml_diff>
--- a/requirements.xlsx
+++ b/requirements.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="10320" windowHeight="3675" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="10320" windowHeight="3675" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="requirements" sheetId="1" r:id="rId1"/>
     <sheet name="filter + s.criteria" sheetId="2" r:id="rId2"/>
     <sheet name="sidebar" sheetId="3" r:id="rId3"/>
     <sheet name="home" sheetId="4" r:id="rId4"/>
+    <sheet name="album view 1" sheetId="5" r:id="rId5"/>
+    <sheet name="album view 2" sheetId="9" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -140,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="107">
   <si>
     <t>Warnings</t>
   </si>
@@ -377,13 +380,97 @@
   </si>
   <si>
     <t>Locations</t>
+  </si>
+  <si>
+    <t>Karnivool</t>
+  </si>
+  <si>
+    <t>01. Simple Boy</t>
+  </si>
+  <si>
+    <t>02. Goliath</t>
+  </si>
+  <si>
+    <t>03. New Day</t>
+  </si>
+  <si>
+    <t>04. Set Fire To The Hive</t>
+  </si>
+  <si>
+    <t>05. Umbra</t>
+  </si>
+  <si>
+    <t>06. All I Know</t>
+  </si>
+  <si>
+    <t>07. The Medicine Wears Off</t>
+  </si>
+  <si>
+    <t>08. The Caudal Lure</t>
+  </si>
+  <si>
+    <t>09. Illumine</t>
+  </si>
+  <si>
+    <t>10. Deadman</t>
+  </si>
+  <si>
+    <t>11. Change</t>
+  </si>
+  <si>
+    <t>Disc 1</t>
+  </si>
+  <si>
+    <t>Total Length: 72:09</t>
+  </si>
+  <si>
+    <t>Format: mp3</t>
+  </si>
+  <si>
+    <t>Size: 138 MB</t>
+  </si>
+  <si>
+    <t>Avg. Bitrate: 265 kbps</t>
+  </si>
+  <si>
+    <t>Sound Awake (2009)</t>
+  </si>
+  <si>
+    <t>72:09, 138 MB, mp3, 265 kbps</t>
+  </si>
+  <si>
+    <t>01. Set Fire To The Hive</t>
+  </si>
+  <si>
+    <t>02. Umbra</t>
+  </si>
+  <si>
+    <t>03. Illumine</t>
+  </si>
+  <si>
+    <t>04. The Medicine Wears Off</t>
+  </si>
+  <si>
+    <t>05. Change</t>
+  </si>
+  <si>
+    <t>06. New Day</t>
+  </si>
+  <si>
+    <t>07. The Caudal Lure</t>
+  </si>
+  <si>
+    <t>125:09, 204 MB, mp3, 265 kbps</t>
+  </si>
+  <si>
+    <t>Disc 2 - Bonus Material</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -443,6 +530,50 @@
     </font>
     <font>
       <sz val="48"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -640,7 +771,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -677,6 +808,36 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="20" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,6 +845,244 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>72429</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Front.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="247650" y="876301"/>
+          <a:ext cx="1885950" cy="1882178"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>225490</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Front.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="333375" y="3381375"/>
+          <a:ext cx="3206815" cy="3200400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>72429</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Front.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="333375" y="895351"/>
+          <a:ext cx="1885950" cy="1882178"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>130507</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Front.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="342900" y="3467100"/>
+          <a:ext cx="3340432" cy="3333750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>130507</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Front.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="342900" y="3657600"/>
+          <a:ext cx="3340432" cy="3333750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>130507</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="Front.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="342900" y="7562850"/>
+          <a:ext cx="3340432" cy="3333750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2171,7 +2570,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:S17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15"/>
   <sheetData>
@@ -2292,4 +2693,2288 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:X35"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.85546875" style="36" customWidth="1"/>
+    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="3" customHeight="1"/>
+    <row r="2" spans="1:18" ht="15" customHeight="1">
+      <c r="A2" s="36">
+        <f>A1+1</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+    </row>
+    <row r="3" spans="1:18" ht="15" customHeight="1">
+      <c r="A3" s="36">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+    </row>
+    <row r="4" spans="1:18" ht="15" customHeight="1">
+      <c r="A4" s="36">
+        <f t="shared" ref="A4:A36" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+    </row>
+    <row r="5" spans="1:18" ht="15" customHeight="1">
+      <c r="A5" s="36">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="36">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="K6" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="27">
+        <v>0.24097222222222223</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="36">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="K7" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="27">
+        <v>0.19305555555555554</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="36">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="K8" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="26"/>
+      <c r="R8" s="27">
+        <v>0.34791666666666665</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="36">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="K9" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="26"/>
+      <c r="R9" s="27">
+        <v>0.18611111111111112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="36">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K10" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="26"/>
+      <c r="P10" s="26"/>
+      <c r="Q10" s="26"/>
+      <c r="R10" s="27">
+        <v>0.32708333333333334</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="36">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="K11" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="27">
+        <v>0.20416666666666669</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="36">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="K12" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="26"/>
+      <c r="R12" s="27">
+        <v>7.6388888888888895E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="36">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="K13" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="26"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="27">
+        <v>0.26111111111111113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="36">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="K14" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
+      <c r="Q14" s="26"/>
+      <c r="R14" s="27">
+        <v>0.21736111111111112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="36">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="K15" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="26"/>
+      <c r="R15" s="27">
+        <v>0.50277777777777777</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="36">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K16" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="26"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26"/>
+      <c r="Q16" s="26"/>
+      <c r="R16" s="27">
+        <v>0.44930555555555557</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24">
+      <c r="A17" s="36">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" ht="22.5" customHeight="1">
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
+    </row>
+    <row r="19" spans="1:24">
+      <c r="A19" s="36">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P19" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q19" s="35"/>
+      <c r="R19" s="35"/>
+      <c r="S19" s="35"/>
+      <c r="T19" s="35"/>
+      <c r="U19" s="35"/>
+      <c r="V19" s="35"/>
+      <c r="W19" s="35"/>
+      <c r="X19" s="35"/>
+    </row>
+    <row r="20" spans="1:24">
+      <c r="A20" s="36">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="P20" s="35"/>
+      <c r="Q20" s="35"/>
+      <c r="R20" s="35"/>
+      <c r="S20" s="35"/>
+      <c r="T20" s="35"/>
+      <c r="U20" s="35"/>
+      <c r="V20" s="35"/>
+      <c r="W20" s="35"/>
+      <c r="X20" s="35"/>
+    </row>
+    <row r="21" spans="1:24">
+      <c r="A21" s="36">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="P21" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q21" s="35"/>
+      <c r="R21" s="35"/>
+      <c r="S21" s="35"/>
+      <c r="T21" s="35"/>
+      <c r="U21" s="35"/>
+      <c r="V21" s="35"/>
+      <c r="W21" s="35"/>
+      <c r="X21" s="35"/>
+    </row>
+    <row r="22" spans="1:24">
+      <c r="A22" s="36">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="P22" s="35"/>
+      <c r="Q22" s="35"/>
+      <c r="R22" s="35"/>
+      <c r="S22" s="35"/>
+      <c r="T22" s="35"/>
+      <c r="U22" s="35"/>
+      <c r="V22" s="35"/>
+      <c r="W22" s="35"/>
+      <c r="X22" s="35"/>
+    </row>
+    <row r="23" spans="1:24">
+      <c r="A23" s="36">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24">
+      <c r="A24" s="36">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="P24" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q24" s="37"/>
+      <c r="R24" s="37"/>
+      <c r="S24" s="37"/>
+      <c r="T24" s="37"/>
+      <c r="U24" s="37"/>
+      <c r="V24" s="37"/>
+      <c r="W24" s="38">
+        <v>0.24097222222222223</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24">
+      <c r="A25" s="36">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="P25" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q25" s="26"/>
+      <c r="R25" s="26"/>
+      <c r="S25" s="26"/>
+      <c r="T25" s="26"/>
+      <c r="U25" s="26"/>
+      <c r="V25" s="26"/>
+      <c r="W25" s="27">
+        <v>0.19305555555555554</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24">
+      <c r="A26" s="36">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="P26" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q26" s="26"/>
+      <c r="R26" s="26"/>
+      <c r="S26" s="26"/>
+      <c r="T26" s="26"/>
+      <c r="U26" s="26"/>
+      <c r="V26" s="26"/>
+      <c r="W26" s="27">
+        <v>0.34791666666666665</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24">
+      <c r="A27" s="36">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="P27" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q27" s="26"/>
+      <c r="R27" s="26"/>
+      <c r="S27" s="26"/>
+      <c r="T27" s="26"/>
+      <c r="U27" s="26"/>
+      <c r="V27" s="26"/>
+      <c r="W27" s="27">
+        <v>0.18611111111111112</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24">
+      <c r="A28" s="36">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="P28" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q28" s="26"/>
+      <c r="R28" s="26"/>
+      <c r="S28" s="26"/>
+      <c r="T28" s="26"/>
+      <c r="U28" s="26"/>
+      <c r="V28" s="26"/>
+      <c r="W28" s="27">
+        <v>0.32708333333333334</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24">
+      <c r="A29" s="36">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="P29" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q29" s="26"/>
+      <c r="R29" s="26"/>
+      <c r="S29" s="26"/>
+      <c r="T29" s="26"/>
+      <c r="U29" s="26"/>
+      <c r="V29" s="26"/>
+      <c r="W29" s="27">
+        <v>0.20416666666666669</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24">
+      <c r="A30" s="36">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="P30" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q30" s="26"/>
+      <c r="R30" s="26"/>
+      <c r="S30" s="26"/>
+      <c r="T30" s="26"/>
+      <c r="U30" s="26"/>
+      <c r="V30" s="26"/>
+      <c r="W30" s="27">
+        <v>7.6388888888888895E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24">
+      <c r="A31" s="36">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="P31" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q31" s="26"/>
+      <c r="R31" s="26"/>
+      <c r="S31" s="26"/>
+      <c r="T31" s="26"/>
+      <c r="U31" s="26"/>
+      <c r="V31" s="26"/>
+      <c r="W31" s="27">
+        <v>0.26111111111111113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24">
+      <c r="A32" s="36">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="P32" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q32" s="26"/>
+      <c r="R32" s="26"/>
+      <c r="S32" s="26"/>
+      <c r="T32" s="26"/>
+      <c r="U32" s="26"/>
+      <c r="V32" s="26"/>
+      <c r="W32" s="27">
+        <v>0.21736111111111112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23">
+      <c r="A33" s="36">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="P33" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q33" s="26"/>
+      <c r="R33" s="26"/>
+      <c r="S33" s="26"/>
+      <c r="T33" s="26"/>
+      <c r="U33" s="26"/>
+      <c r="V33" s="26"/>
+      <c r="W33" s="27">
+        <v>0.50277777777777777</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23">
+      <c r="A34" s="36">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="P34" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q34" s="28"/>
+      <c r="R34" s="28"/>
+      <c r="S34" s="28"/>
+      <c r="T34" s="28"/>
+      <c r="U34" s="28"/>
+      <c r="V34" s="28"/>
+      <c r="W34" s="42">
+        <v>0.44930555555555557</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23">
+      <c r="A35" s="36">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="W35" s="40" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:J3"/>
+    <mergeCell ref="B4:J5"/>
+    <mergeCell ref="P19:X20"/>
+    <mergeCell ref="P21:X22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AF76"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="V39" sqref="V39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.85546875" style="36" customWidth="1"/>
+    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.7109375" customWidth="1"/>
+    <col min="32" max="32" width="4.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" ht="3" customHeight="1"/>
+    <row r="2" spans="1:27" ht="15" customHeight="1">
+      <c r="A2" s="36">
+        <f>A1+1</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+    </row>
+    <row r="3" spans="1:27" ht="15" customHeight="1">
+      <c r="A3" s="36">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+    </row>
+    <row r="4" spans="1:27" ht="15" customHeight="1">
+      <c r="A4" s="36">
+        <f t="shared" ref="A4:A38" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+    </row>
+    <row r="5" spans="1:27" ht="15" customHeight="1">
+      <c r="A5" s="36">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+    </row>
+    <row r="6" spans="1:27">
+      <c r="A6" s="36">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="K6" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="T6" s="39" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27">
+      <c r="A7" s="36">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="K7" s="6"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="T7" s="6"/>
+      <c r="U7" s="28"/>
+      <c r="V7" s="28"/>
+      <c r="W7" s="28"/>
+      <c r="X7" s="28"/>
+      <c r="Y7" s="28"/>
+      <c r="Z7" s="28"/>
+      <c r="AA7" s="30" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27">
+      <c r="A8" s="36">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="K8" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="26"/>
+      <c r="R8" s="27">
+        <v>0.24097222222222223</v>
+      </c>
+      <c r="T8" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="U8" s="26"/>
+      <c r="V8" s="26"/>
+      <c r="W8" s="26"/>
+      <c r="X8" s="26"/>
+      <c r="Y8" s="26"/>
+      <c r="Z8" s="26"/>
+      <c r="AA8" s="27">
+        <v>0.24097222222222223</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27">
+      <c r="A9" s="36">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="K9" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="26"/>
+      <c r="R9" s="27">
+        <v>0.19305555555555554</v>
+      </c>
+      <c r="T9" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="U9" s="26"/>
+      <c r="V9" s="26"/>
+      <c r="W9" s="26"/>
+      <c r="X9" s="26"/>
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="26"/>
+      <c r="AA9" s="27">
+        <v>0.19305555555555554</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27">
+      <c r="A10" s="36">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K10" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="26"/>
+      <c r="P10" s="26"/>
+      <c r="Q10" s="26"/>
+      <c r="R10" s="27">
+        <v>0.34791666666666665</v>
+      </c>
+      <c r="T10" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="U10" s="26"/>
+      <c r="V10" s="26"/>
+      <c r="W10" s="26"/>
+      <c r="X10" s="26"/>
+      <c r="Y10" s="26"/>
+      <c r="Z10" s="26"/>
+      <c r="AA10" s="27">
+        <v>0.34791666666666665</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27">
+      <c r="A11" s="36">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="K11" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="27">
+        <v>0.18611111111111112</v>
+      </c>
+      <c r="T11" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="U11" s="26"/>
+      <c r="V11" s="26"/>
+      <c r="W11" s="26"/>
+      <c r="X11" s="26"/>
+      <c r="Y11" s="26"/>
+      <c r="Z11" s="26"/>
+      <c r="AA11" s="27">
+        <v>0.18611111111111112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27">
+      <c r="A12" s="36">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="K12" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="26"/>
+      <c r="R12" s="27">
+        <v>0.32708333333333334</v>
+      </c>
+      <c r="T12" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="U12" s="26"/>
+      <c r="V12" s="26"/>
+      <c r="W12" s="26"/>
+      <c r="X12" s="26"/>
+      <c r="Y12" s="26"/>
+      <c r="Z12" s="26"/>
+      <c r="AA12" s="27">
+        <v>0.32708333333333334</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27">
+      <c r="A13" s="36">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="K13" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="26"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="27">
+        <v>0.20416666666666669</v>
+      </c>
+      <c r="T13" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="U13" s="26"/>
+      <c r="V13" s="26"/>
+      <c r="W13" s="26"/>
+      <c r="X13" s="26"/>
+      <c r="Y13" s="26"/>
+      <c r="Z13" s="26"/>
+      <c r="AA13" s="27">
+        <v>0.20416666666666669</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27">
+      <c r="A14" s="36">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="K14" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
+      <c r="Q14" s="26"/>
+      <c r="R14" s="27">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="T14" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="U14" s="26"/>
+      <c r="V14" s="26"/>
+      <c r="W14" s="26"/>
+      <c r="X14" s="26"/>
+      <c r="Y14" s="26"/>
+      <c r="Z14" s="26"/>
+      <c r="AA14" s="27">
+        <v>7.6388888888888895E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27">
+      <c r="A15" s="36">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="K15" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="26"/>
+      <c r="R15" s="27">
+        <v>0.26111111111111113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27">
+      <c r="A16" s="36">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K16" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="26"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26"/>
+      <c r="Q16" s="26"/>
+      <c r="R16" s="27">
+        <v>0.21736111111111112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32">
+      <c r="A17" s="36">
+        <f>A15+1</f>
+        <v>15</v>
+      </c>
+      <c r="K17" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="26"/>
+      <c r="R17" s="27">
+        <v>0.50277777777777777</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32">
+      <c r="A18" s="36">
+        <f>A16+1</f>
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>105</v>
+      </c>
+      <c r="K18" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="26"/>
+      <c r="O18" s="26"/>
+      <c r="P18" s="26"/>
+      <c r="Q18" s="26"/>
+      <c r="R18" s="27">
+        <v>0.44930555555555557</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" ht="22.5" customHeight="1">
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="26"/>
+    </row>
+    <row r="20" spans="1:32">
+      <c r="A20" s="36">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P20" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q20" s="33"/>
+      <c r="R20" s="33"/>
+      <c r="S20" s="33"/>
+      <c r="T20" s="33"/>
+      <c r="U20" s="33"/>
+      <c r="V20" s="33"/>
+      <c r="W20" s="33"/>
+      <c r="X20" s="33"/>
+    </row>
+    <row r="21" spans="1:32">
+      <c r="A21" s="36">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="P21" s="33"/>
+      <c r="Q21" s="33"/>
+      <c r="R21" s="33"/>
+      <c r="S21" s="33"/>
+      <c r="T21" s="33"/>
+      <c r="U21" s="33"/>
+      <c r="V21" s="33"/>
+      <c r="W21" s="33"/>
+      <c r="X21" s="33"/>
+    </row>
+    <row r="22" spans="1:32">
+      <c r="A22" s="36">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="P22" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q22" s="35"/>
+      <c r="R22" s="35"/>
+      <c r="S22" s="35"/>
+      <c r="T22" s="35"/>
+      <c r="U22" s="35"/>
+      <c r="V22" s="35"/>
+      <c r="W22" s="35"/>
+      <c r="X22" s="35"/>
+    </row>
+    <row r="23" spans="1:32">
+      <c r="A23" s="36">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="P23" s="35"/>
+      <c r="Q23" s="35"/>
+      <c r="R23" s="35"/>
+      <c r="S23" s="35"/>
+      <c r="T23" s="35"/>
+      <c r="U23" s="35"/>
+      <c r="V23" s="35"/>
+      <c r="W23" s="35"/>
+      <c r="X23" s="35"/>
+    </row>
+    <row r="24" spans="1:32">
+      <c r="A24" s="36">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="P24" s="31" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32">
+      <c r="A25" s="36">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32">
+      <c r="A26" s="36">
+        <f>A23+1</f>
+        <v>5</v>
+      </c>
+      <c r="P26" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y26" s="39" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:32">
+      <c r="A27" s="36">
+        <f>A24+1</f>
+        <v>6</v>
+      </c>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="28"/>
+      <c r="R27" s="28"/>
+      <c r="S27" s="28"/>
+      <c r="T27" s="28"/>
+      <c r="U27" s="28"/>
+      <c r="V27" s="28"/>
+      <c r="W27" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y27" s="6"/>
+      <c r="Z27" s="28"/>
+      <c r="AA27" s="28"/>
+      <c r="AB27" s="28"/>
+      <c r="AC27" s="28"/>
+      <c r="AD27" s="28"/>
+      <c r="AE27" s="28"/>
+      <c r="AF27" s="30" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32">
+      <c r="A28" s="36">
+        <f>A25+1</f>
+        <v>7</v>
+      </c>
+      <c r="P28" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q28" s="37"/>
+      <c r="R28" s="37"/>
+      <c r="S28" s="37"/>
+      <c r="T28" s="37"/>
+      <c r="U28" s="37"/>
+      <c r="V28" s="37"/>
+      <c r="W28" s="38">
+        <v>0.24097222222222223</v>
+      </c>
+      <c r="Y28" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z28" s="26"/>
+      <c r="AA28" s="26"/>
+      <c r="AB28" s="26"/>
+      <c r="AC28" s="26"/>
+      <c r="AD28" s="26"/>
+      <c r="AE28" s="26"/>
+      <c r="AF28" s="27">
+        <v>0.24097222222222223</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32">
+      <c r="A29" s="36">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="P29" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q29" s="26"/>
+      <c r="R29" s="26"/>
+      <c r="S29" s="26"/>
+      <c r="T29" s="26"/>
+      <c r="U29" s="26"/>
+      <c r="V29" s="26"/>
+      <c r="W29" s="27">
+        <v>0.19305555555555554</v>
+      </c>
+      <c r="Y29" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z29" s="26"/>
+      <c r="AA29" s="26"/>
+      <c r="AB29" s="26"/>
+      <c r="AC29" s="26"/>
+      <c r="AD29" s="26"/>
+      <c r="AE29" s="26"/>
+      <c r="AF29" s="27">
+        <v>0.19305555555555554</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32">
+      <c r="A30" s="36">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="P30" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q30" s="26"/>
+      <c r="R30" s="26"/>
+      <c r="S30" s="26"/>
+      <c r="T30" s="26"/>
+      <c r="U30" s="26"/>
+      <c r="V30" s="26"/>
+      <c r="W30" s="27">
+        <v>0.34791666666666665</v>
+      </c>
+      <c r="Y30" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z30" s="26"/>
+      <c r="AA30" s="26"/>
+      <c r="AB30" s="26"/>
+      <c r="AC30" s="26"/>
+      <c r="AD30" s="26"/>
+      <c r="AE30" s="26"/>
+      <c r="AF30" s="27">
+        <v>0.34791666666666665</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32">
+      <c r="A31" s="36">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="P31" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q31" s="26"/>
+      <c r="R31" s="26"/>
+      <c r="S31" s="26"/>
+      <c r="T31" s="26"/>
+      <c r="U31" s="26"/>
+      <c r="V31" s="26"/>
+      <c r="W31" s="27">
+        <v>0.18611111111111112</v>
+      </c>
+      <c r="Y31" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z31" s="26"/>
+      <c r="AA31" s="26"/>
+      <c r="AB31" s="26"/>
+      <c r="AC31" s="26"/>
+      <c r="AD31" s="26"/>
+      <c r="AE31" s="26"/>
+      <c r="AF31" s="27">
+        <v>0.18611111111111112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32">
+      <c r="A32" s="36">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="P32" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q32" s="26"/>
+      <c r="R32" s="26"/>
+      <c r="S32" s="26"/>
+      <c r="T32" s="26"/>
+      <c r="U32" s="26"/>
+      <c r="V32" s="26"/>
+      <c r="W32" s="27">
+        <v>0.32708333333333334</v>
+      </c>
+      <c r="Y32" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z32" s="26"/>
+      <c r="AA32" s="26"/>
+      <c r="AB32" s="26"/>
+      <c r="AC32" s="26"/>
+      <c r="AD32" s="26"/>
+      <c r="AE32" s="26"/>
+      <c r="AF32" s="27">
+        <v>0.32708333333333334</v>
+      </c>
+    </row>
+    <row r="33" spans="1:32">
+      <c r="A33" s="36">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="P33" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q33" s="26"/>
+      <c r="R33" s="26"/>
+      <c r="S33" s="26"/>
+      <c r="T33" s="26"/>
+      <c r="U33" s="26"/>
+      <c r="V33" s="26"/>
+      <c r="W33" s="27">
+        <v>0.20416666666666669</v>
+      </c>
+      <c r="Y33" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z33" s="26"/>
+      <c r="AA33" s="26"/>
+      <c r="AB33" s="26"/>
+      <c r="AC33" s="26"/>
+      <c r="AD33" s="26"/>
+      <c r="AE33" s="26"/>
+      <c r="AF33" s="27">
+        <v>0.20416666666666669</v>
+      </c>
+    </row>
+    <row r="34" spans="1:32">
+      <c r="A34" s="36">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="P34" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q34" s="26"/>
+      <c r="R34" s="26"/>
+      <c r="S34" s="26"/>
+      <c r="T34" s="26"/>
+      <c r="U34" s="26"/>
+      <c r="V34" s="26"/>
+      <c r="W34" s="27">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="Y34" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z34" s="26"/>
+      <c r="AA34" s="26"/>
+      <c r="AB34" s="26"/>
+      <c r="AC34" s="26"/>
+      <c r="AD34" s="26"/>
+      <c r="AE34" s="26"/>
+      <c r="AF34" s="27">
+        <v>7.6388888888888895E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:32">
+      <c r="A35" s="36">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="P35" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q35" s="26"/>
+      <c r="R35" s="26"/>
+      <c r="S35" s="26"/>
+      <c r="T35" s="26"/>
+      <c r="U35" s="26"/>
+      <c r="V35" s="26"/>
+      <c r="W35" s="27">
+        <v>0.26111111111111113</v>
+      </c>
+    </row>
+    <row r="36" spans="1:32">
+      <c r="A36" s="36">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="P36" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q36" s="26"/>
+      <c r="R36" s="26"/>
+      <c r="S36" s="26"/>
+      <c r="T36" s="26"/>
+      <c r="U36" s="26"/>
+      <c r="V36" s="26"/>
+      <c r="W36" s="27">
+        <v>0.21736111111111112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:32">
+      <c r="A37" s="36">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="P37" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q37" s="26"/>
+      <c r="R37" s="26"/>
+      <c r="S37" s="26"/>
+      <c r="T37" s="26"/>
+      <c r="U37" s="26"/>
+      <c r="V37" s="26"/>
+      <c r="W37" s="27">
+        <v>0.50277777777777777</v>
+      </c>
+    </row>
+    <row r="38" spans="1:32">
+      <c r="A38" s="36">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="P38" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q38" s="26"/>
+      <c r="R38" s="26"/>
+      <c r="S38" s="26"/>
+      <c r="T38" s="26"/>
+      <c r="U38" s="26"/>
+      <c r="V38" s="26"/>
+      <c r="W38" s="27">
+        <v>0.44930555555555557</v>
+      </c>
+    </row>
+    <row r="39" spans="1:32" ht="22.5" customHeight="1">
+      <c r="K39" s="26"/>
+      <c r="L39" s="26"/>
+      <c r="M39" s="26"/>
+    </row>
+    <row r="40" spans="1:32">
+      <c r="A40" s="36">
+        <f t="shared" ref="A40:A46" si="1">A39+1</f>
+        <v>1</v>
+      </c>
+      <c r="P40" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q40" s="33"/>
+      <c r="R40" s="33"/>
+      <c r="S40" s="33"/>
+      <c r="T40" s="33"/>
+      <c r="U40" s="33"/>
+      <c r="V40" s="33"/>
+      <c r="W40" s="33"/>
+      <c r="X40" s="33"/>
+    </row>
+    <row r="41" spans="1:32">
+      <c r="A41" s="36">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="P41" s="33"/>
+      <c r="Q41" s="33"/>
+      <c r="R41" s="33"/>
+      <c r="S41" s="33"/>
+      <c r="T41" s="33"/>
+      <c r="U41" s="33"/>
+      <c r="V41" s="33"/>
+      <c r="W41" s="33"/>
+      <c r="X41" s="33"/>
+    </row>
+    <row r="42" spans="1:32">
+      <c r="A42" s="36">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="P42" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q42" s="35"/>
+      <c r="R42" s="35"/>
+      <c r="S42" s="35"/>
+      <c r="T42" s="35"/>
+      <c r="U42" s="35"/>
+      <c r="V42" s="35"/>
+      <c r="W42" s="35"/>
+      <c r="X42" s="35"/>
+    </row>
+    <row r="43" spans="1:32">
+      <c r="A43" s="36">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="P43" s="35"/>
+      <c r="Q43" s="35"/>
+      <c r="R43" s="35"/>
+      <c r="S43" s="35"/>
+      <c r="T43" s="35"/>
+      <c r="U43" s="35"/>
+      <c r="V43" s="35"/>
+      <c r="W43" s="35"/>
+      <c r="X43" s="35"/>
+    </row>
+    <row r="44" spans="1:32">
+      <c r="A44" s="36">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:32">
+      <c r="A45" s="36">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="P45" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y45" s="39" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="46" spans="1:32">
+      <c r="A46" s="36">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="P46" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q46" s="37"/>
+      <c r="R46" s="37"/>
+      <c r="S46" s="37"/>
+      <c r="T46" s="37"/>
+      <c r="U46" s="37"/>
+      <c r="V46" s="37"/>
+      <c r="W46" s="38">
+        <v>0.24097222222222223</v>
+      </c>
+      <c r="Y46" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z46" s="37"/>
+      <c r="AA46" s="37"/>
+      <c r="AB46" s="37"/>
+      <c r="AC46" s="37"/>
+      <c r="AD46" s="37"/>
+      <c r="AE46" s="37"/>
+      <c r="AF46" s="38">
+        <v>0.24097222222222223</v>
+      </c>
+    </row>
+    <row r="47" spans="1:32">
+      <c r="A47" s="36">
+        <f>A44+1</f>
+        <v>6</v>
+      </c>
+      <c r="P47" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q47" s="26"/>
+      <c r="R47" s="26"/>
+      <c r="S47" s="26"/>
+      <c r="T47" s="26"/>
+      <c r="U47" s="26"/>
+      <c r="V47" s="26"/>
+      <c r="W47" s="27">
+        <v>0.19305555555555554</v>
+      </c>
+      <c r="Y47" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z47" s="29"/>
+      <c r="AA47" s="29"/>
+      <c r="AB47" s="29"/>
+      <c r="AC47" s="29"/>
+      <c r="AD47" s="29"/>
+      <c r="AE47" s="29"/>
+      <c r="AF47" s="41">
+        <v>0.19305555555555554</v>
+      </c>
+    </row>
+    <row r="48" spans="1:32">
+      <c r="A48" s="36">
+        <f t="shared" ref="A48:A57" si="2">A47+1</f>
+        <v>7</v>
+      </c>
+      <c r="P48" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q48" s="26"/>
+      <c r="R48" s="26"/>
+      <c r="S48" s="26"/>
+      <c r="T48" s="26"/>
+      <c r="U48" s="26"/>
+      <c r="V48" s="26"/>
+      <c r="W48" s="27">
+        <v>0.34791666666666665</v>
+      </c>
+      <c r="Y48" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z48" s="29"/>
+      <c r="AA48" s="29"/>
+      <c r="AB48" s="29"/>
+      <c r="AC48" s="29"/>
+      <c r="AD48" s="29"/>
+      <c r="AE48" s="29"/>
+      <c r="AF48" s="41">
+        <v>0.34791666666666665</v>
+      </c>
+    </row>
+    <row r="49" spans="1:32">
+      <c r="A49" s="36">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="P49" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q49" s="26"/>
+      <c r="R49" s="26"/>
+      <c r="S49" s="26"/>
+      <c r="T49" s="26"/>
+      <c r="U49" s="26"/>
+      <c r="V49" s="26"/>
+      <c r="W49" s="27">
+        <v>0.18611111111111112</v>
+      </c>
+      <c r="Y49" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z49" s="29"/>
+      <c r="AA49" s="29"/>
+      <c r="AB49" s="29"/>
+      <c r="AC49" s="29"/>
+      <c r="AD49" s="29"/>
+      <c r="AE49" s="29"/>
+      <c r="AF49" s="41">
+        <v>0.18611111111111112</v>
+      </c>
+    </row>
+    <row r="50" spans="1:32">
+      <c r="A50" s="36">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="P50" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q50" s="26"/>
+      <c r="R50" s="26"/>
+      <c r="S50" s="26"/>
+      <c r="T50" s="26"/>
+      <c r="U50" s="26"/>
+      <c r="V50" s="26"/>
+      <c r="W50" s="27">
+        <v>0.32708333333333334</v>
+      </c>
+      <c r="Y50" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z50" s="29"/>
+      <c r="AA50" s="29"/>
+      <c r="AB50" s="29"/>
+      <c r="AC50" s="29"/>
+      <c r="AD50" s="29"/>
+      <c r="AE50" s="29"/>
+      <c r="AF50" s="41">
+        <v>0.32708333333333334</v>
+      </c>
+    </row>
+    <row r="51" spans="1:32">
+      <c r="A51" s="36">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="P51" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q51" s="26"/>
+      <c r="R51" s="26"/>
+      <c r="S51" s="26"/>
+      <c r="T51" s="26"/>
+      <c r="U51" s="26"/>
+      <c r="V51" s="26"/>
+      <c r="W51" s="27">
+        <v>0.20416666666666669</v>
+      </c>
+      <c r="Y51" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z51" s="29"/>
+      <c r="AA51" s="29"/>
+      <c r="AB51" s="29"/>
+      <c r="AC51" s="29"/>
+      <c r="AD51" s="29"/>
+      <c r="AE51" s="29"/>
+      <c r="AF51" s="41">
+        <v>0.20416666666666669</v>
+      </c>
+    </row>
+    <row r="52" spans="1:32">
+      <c r="A52" s="36">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="P52" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q52" s="26"/>
+      <c r="R52" s="26"/>
+      <c r="S52" s="26"/>
+      <c r="T52" s="26"/>
+      <c r="U52" s="26"/>
+      <c r="V52" s="26"/>
+      <c r="W52" s="27">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="Y52" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z52" s="29"/>
+      <c r="AA52" s="29"/>
+      <c r="AB52" s="29"/>
+      <c r="AC52" s="29"/>
+      <c r="AD52" s="29"/>
+      <c r="AE52" s="29"/>
+      <c r="AF52" s="41">
+        <v>7.6388888888888895E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:32">
+      <c r="A53" s="36">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="P53" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q53" s="26"/>
+      <c r="R53" s="26"/>
+      <c r="S53" s="26"/>
+      <c r="T53" s="26"/>
+      <c r="U53" s="26"/>
+      <c r="V53" s="26"/>
+      <c r="W53" s="27">
+        <v>0.26111111111111113</v>
+      </c>
+      <c r="Y53" s="8"/>
+      <c r="Z53" s="8"/>
+      <c r="AA53" s="8"/>
+      <c r="AB53" s="8"/>
+      <c r="AC53" s="8"/>
+      <c r="AD53" s="8"/>
+      <c r="AE53" s="8"/>
+      <c r="AF53" s="8"/>
+    </row>
+    <row r="54" spans="1:32">
+      <c r="A54" s="36">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="P54" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q54" s="26"/>
+      <c r="R54" s="26"/>
+      <c r="S54" s="26"/>
+      <c r="T54" s="26"/>
+      <c r="U54" s="26"/>
+      <c r="V54" s="26"/>
+      <c r="W54" s="27">
+        <v>0.21736111111111112</v>
+      </c>
+      <c r="Y54" s="8"/>
+      <c r="Z54" s="8"/>
+      <c r="AA54" s="8"/>
+      <c r="AB54" s="8"/>
+      <c r="AC54" s="8"/>
+      <c r="AD54" s="8"/>
+      <c r="AE54" s="8"/>
+      <c r="AF54" s="8"/>
+    </row>
+    <row r="55" spans="1:32">
+      <c r="A55" s="36">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="P55" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q55" s="26"/>
+      <c r="R55" s="26"/>
+      <c r="S55" s="26"/>
+      <c r="T55" s="26"/>
+      <c r="U55" s="26"/>
+      <c r="V55" s="26"/>
+      <c r="W55" s="27">
+        <v>0.50277777777777777</v>
+      </c>
+      <c r="Y55" s="8"/>
+      <c r="Z55" s="8"/>
+      <c r="AA55" s="8"/>
+      <c r="AB55" s="8"/>
+      <c r="AC55" s="8"/>
+      <c r="AD55" s="8"/>
+      <c r="AE55" s="8"/>
+      <c r="AF55" s="8"/>
+    </row>
+    <row r="56" spans="1:32">
+      <c r="A56" s="36">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="P56" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q56" s="26"/>
+      <c r="R56" s="26"/>
+      <c r="S56" s="26"/>
+      <c r="T56" s="26"/>
+      <c r="U56" s="26"/>
+      <c r="V56" s="26"/>
+      <c r="W56" s="27">
+        <v>0.44930555555555557</v>
+      </c>
+      <c r="Y56" s="6"/>
+      <c r="Z56" s="6"/>
+      <c r="AA56" s="6"/>
+      <c r="AB56" s="6"/>
+      <c r="AC56" s="6"/>
+      <c r="AD56" s="6"/>
+      <c r="AE56" s="6"/>
+      <c r="AF56" s="6"/>
+    </row>
+    <row r="57" spans="1:32">
+      <c r="A57" s="36">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="P57" s="17"/>
+      <c r="Q57" s="17"/>
+      <c r="R57" s="17"/>
+      <c r="S57" s="17"/>
+      <c r="T57" s="17"/>
+      <c r="U57" s="17"/>
+      <c r="V57" s="17"/>
+      <c r="W57" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="AF57" s="43" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="58" spans="1:32" ht="22.5" customHeight="1">
+      <c r="K58" s="26"/>
+      <c r="L58" s="26"/>
+      <c r="M58" s="26"/>
+    </row>
+    <row r="59" spans="1:32">
+      <c r="A59" s="36">
+        <f t="shared" ref="A59:A65" si="3">A58+1</f>
+        <v>1</v>
+      </c>
+      <c r="P59" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q59" s="33"/>
+      <c r="R59" s="33"/>
+      <c r="S59" s="33"/>
+      <c r="T59" s="33"/>
+      <c r="U59" s="33"/>
+      <c r="V59" s="33"/>
+      <c r="W59" s="33"/>
+      <c r="X59" s="33"/>
+    </row>
+    <row r="60" spans="1:32">
+      <c r="A60" s="36">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="P60" s="33"/>
+      <c r="Q60" s="33"/>
+      <c r="R60" s="33"/>
+      <c r="S60" s="33"/>
+      <c r="T60" s="33"/>
+      <c r="U60" s="33"/>
+      <c r="V60" s="33"/>
+      <c r="W60" s="33"/>
+      <c r="X60" s="33"/>
+    </row>
+    <row r="61" spans="1:32">
+      <c r="A61" s="36">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="P61" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q61" s="35"/>
+      <c r="R61" s="35"/>
+      <c r="S61" s="35"/>
+      <c r="T61" s="35"/>
+      <c r="U61" s="35"/>
+      <c r="V61" s="35"/>
+      <c r="W61" s="35"/>
+      <c r="X61" s="35"/>
+    </row>
+    <row r="62" spans="1:32">
+      <c r="A62" s="36">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="P62" s="35"/>
+      <c r="Q62" s="35"/>
+      <c r="R62" s="35"/>
+      <c r="S62" s="35"/>
+      <c r="T62" s="35"/>
+      <c r="U62" s="35"/>
+      <c r="V62" s="35"/>
+      <c r="W62" s="35"/>
+      <c r="X62" s="35"/>
+    </row>
+    <row r="63" spans="1:32">
+      <c r="A63" s="36">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:32">
+      <c r="A64" s="36">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="P64" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y64" s="39" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="65" spans="1:32">
+      <c r="A65" s="36">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="P65" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q65" s="37"/>
+      <c r="R65" s="37"/>
+      <c r="S65" s="37"/>
+      <c r="T65" s="37"/>
+      <c r="U65" s="37"/>
+      <c r="V65" s="37"/>
+      <c r="W65" s="38">
+        <v>0.24097222222222223</v>
+      </c>
+      <c r="Y65" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z65" s="37"/>
+      <c r="AA65" s="37"/>
+      <c r="AB65" s="37"/>
+      <c r="AC65" s="37"/>
+      <c r="AD65" s="37"/>
+      <c r="AE65" s="37"/>
+      <c r="AF65" s="38">
+        <v>0.24097222222222223</v>
+      </c>
+    </row>
+    <row r="66" spans="1:32">
+      <c r="A66" s="36">
+        <f>A63+1</f>
+        <v>6</v>
+      </c>
+      <c r="P66" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q66" s="26"/>
+      <c r="R66" s="26"/>
+      <c r="S66" s="26"/>
+      <c r="T66" s="26"/>
+      <c r="U66" s="26"/>
+      <c r="V66" s="26"/>
+      <c r="W66" s="27">
+        <v>0.19305555555555554</v>
+      </c>
+      <c r="Y66" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z66" s="29"/>
+      <c r="AA66" s="29"/>
+      <c r="AB66" s="29"/>
+      <c r="AC66" s="29"/>
+      <c r="AD66" s="29"/>
+      <c r="AE66" s="29"/>
+      <c r="AF66" s="41">
+        <v>0.19305555555555554</v>
+      </c>
+    </row>
+    <row r="67" spans="1:32">
+      <c r="A67" s="36">
+        <f t="shared" ref="A67:A76" si="4">A66+1</f>
+        <v>7</v>
+      </c>
+      <c r="P67" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q67" s="26"/>
+      <c r="R67" s="26"/>
+      <c r="S67" s="26"/>
+      <c r="T67" s="26"/>
+      <c r="U67" s="26"/>
+      <c r="V67" s="26"/>
+      <c r="W67" s="27">
+        <v>0.34791666666666665</v>
+      </c>
+      <c r="Y67" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z67" s="29"/>
+      <c r="AA67" s="29"/>
+      <c r="AB67" s="29"/>
+      <c r="AC67" s="29"/>
+      <c r="AD67" s="29"/>
+      <c r="AE67" s="29"/>
+      <c r="AF67" s="41">
+        <v>0.34791666666666665</v>
+      </c>
+    </row>
+    <row r="68" spans="1:32">
+      <c r="A68" s="36">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="P68" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q68" s="26"/>
+      <c r="R68" s="26"/>
+      <c r="S68" s="26"/>
+      <c r="T68" s="26"/>
+      <c r="U68" s="26"/>
+      <c r="V68" s="26"/>
+      <c r="W68" s="27">
+        <v>0.18611111111111112</v>
+      </c>
+      <c r="Y68" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z68" s="29"/>
+      <c r="AA68" s="29"/>
+      <c r="AB68" s="29"/>
+      <c r="AC68" s="29"/>
+      <c r="AD68" s="29"/>
+      <c r="AE68" s="29"/>
+      <c r="AF68" s="41">
+        <v>0.18611111111111112</v>
+      </c>
+    </row>
+    <row r="69" spans="1:32">
+      <c r="A69" s="36">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="P69" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q69" s="26"/>
+      <c r="R69" s="26"/>
+      <c r="S69" s="26"/>
+      <c r="T69" s="26"/>
+      <c r="U69" s="26"/>
+      <c r="V69" s="26"/>
+      <c r="W69" s="27">
+        <v>0.32708333333333334</v>
+      </c>
+      <c r="Y69" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z69" s="29"/>
+      <c r="AA69" s="29"/>
+      <c r="AB69" s="29"/>
+      <c r="AC69" s="29"/>
+      <c r="AD69" s="29"/>
+      <c r="AE69" s="29"/>
+      <c r="AF69" s="41">
+        <v>0.32708333333333334</v>
+      </c>
+    </row>
+    <row r="70" spans="1:32">
+      <c r="A70" s="36">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="P70" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q70" s="26"/>
+      <c r="R70" s="26"/>
+      <c r="S70" s="26"/>
+      <c r="T70" s="26"/>
+      <c r="U70" s="26"/>
+      <c r="V70" s="26"/>
+      <c r="W70" s="27">
+        <v>0.20416666666666669</v>
+      </c>
+      <c r="Y70" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z70" s="29"/>
+      <c r="AA70" s="29"/>
+      <c r="AB70" s="29"/>
+      <c r="AC70" s="29"/>
+      <c r="AD70" s="29"/>
+      <c r="AE70" s="29"/>
+      <c r="AF70" s="41">
+        <v>0.20416666666666669</v>
+      </c>
+    </row>
+    <row r="71" spans="1:32">
+      <c r="A71" s="36">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="P71" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q71" s="26"/>
+      <c r="R71" s="26"/>
+      <c r="S71" s="26"/>
+      <c r="T71" s="26"/>
+      <c r="U71" s="26"/>
+      <c r="V71" s="26"/>
+      <c r="W71" s="27">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="Y71" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z71" s="29"/>
+      <c r="AA71" s="29"/>
+      <c r="AB71" s="29"/>
+      <c r="AC71" s="29"/>
+      <c r="AD71" s="29"/>
+      <c r="AE71" s="29"/>
+      <c r="AF71" s="41">
+        <v>7.6388888888888895E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:32">
+      <c r="A72" s="36">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="P72" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q72" s="26"/>
+      <c r="R72" s="26"/>
+      <c r="S72" s="26"/>
+      <c r="T72" s="26"/>
+      <c r="U72" s="26"/>
+      <c r="V72" s="26"/>
+      <c r="W72" s="27">
+        <v>0.26111111111111113</v>
+      </c>
+      <c r="Y72" s="17"/>
+      <c r="Z72" s="17"/>
+      <c r="AA72" s="17"/>
+      <c r="AB72" s="17"/>
+      <c r="AC72" s="17"/>
+      <c r="AD72" s="17"/>
+      <c r="AE72" s="17"/>
+      <c r="AF72" s="40" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="73" spans="1:32">
+      <c r="A73" s="36">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="P73" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q73" s="26"/>
+      <c r="R73" s="26"/>
+      <c r="S73" s="26"/>
+      <c r="T73" s="26"/>
+      <c r="U73" s="26"/>
+      <c r="V73" s="26"/>
+      <c r="W73" s="27">
+        <v>0.21736111111111112</v>
+      </c>
+      <c r="Y73" s="8"/>
+      <c r="Z73" s="8"/>
+      <c r="AA73" s="8"/>
+      <c r="AB73" s="8"/>
+      <c r="AC73" s="8"/>
+      <c r="AD73" s="8"/>
+      <c r="AE73" s="8"/>
+      <c r="AF73" s="8"/>
+    </row>
+    <row r="74" spans="1:32">
+      <c r="A74" s="36">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="P74" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q74" s="26"/>
+      <c r="R74" s="26"/>
+      <c r="S74" s="26"/>
+      <c r="T74" s="26"/>
+      <c r="U74" s="26"/>
+      <c r="V74" s="26"/>
+      <c r="W74" s="27">
+        <v>0.50277777777777777</v>
+      </c>
+      <c r="Y74" s="8"/>
+      <c r="Z74" s="8"/>
+      <c r="AA74" s="8"/>
+      <c r="AB74" s="8"/>
+      <c r="AC74" s="8"/>
+      <c r="AD74" s="8"/>
+      <c r="AE74" s="8"/>
+      <c r="AF74" s="8"/>
+    </row>
+    <row r="75" spans="1:32">
+      <c r="A75" s="36">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="P75" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q75" s="26"/>
+      <c r="R75" s="26"/>
+      <c r="S75" s="26"/>
+      <c r="T75" s="26"/>
+      <c r="U75" s="26"/>
+      <c r="V75" s="26"/>
+      <c r="W75" s="27">
+        <v>0.44930555555555557</v>
+      </c>
+      <c r="Y75" s="8"/>
+      <c r="Z75" s="8"/>
+      <c r="AA75" s="8"/>
+      <c r="AB75" s="8"/>
+      <c r="AC75" s="8"/>
+      <c r="AD75" s="8"/>
+      <c r="AE75" s="8"/>
+      <c r="AF75" s="8"/>
+    </row>
+    <row r="76" spans="1:32">
+      <c r="A76" s="36">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="P76" s="17"/>
+      <c r="Q76" s="17"/>
+      <c r="R76" s="17"/>
+      <c r="S76" s="17"/>
+      <c r="T76" s="17"/>
+      <c r="U76" s="17"/>
+      <c r="V76" s="17"/>
+      <c r="W76" s="40" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="P59:X60"/>
+    <mergeCell ref="P61:X62"/>
+    <mergeCell ref="B2:J3"/>
+    <mergeCell ref="B4:J5"/>
+    <mergeCell ref="P20:X21"/>
+    <mergeCell ref="P22:X23"/>
+    <mergeCell ref="P40:X41"/>
+    <mergeCell ref="P42:X43"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added a reset button to the search filter design
</commit_message>
<xml_diff>
--- a/requirements.xlsx
+++ b/requirements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="10320" windowHeight="3675" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="10320" windowHeight="3675" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="requirements" sheetId="1" r:id="rId1"/>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="108">
   <si>
     <t>Warnings</t>
   </si>
@@ -464,6 +464,9 @@
   </si>
   <si>
     <t>Disc 2 - Bonus Material</t>
+  </si>
+  <si>
+    <t>Reset</t>
   </si>
 </sst>
 </file>
@@ -816,14 +819,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -837,6 +832,14 @@
     <xf numFmtId="20" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1797,7 +1800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.85546875" defaultRowHeight="15"/>
   <sheetData>
@@ -2438,16 +2441,16 @@
     <row r="35" spans="1:15">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="12" t="s">
+      <c r="D35" s="11"/>
+      <c r="E35" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="I35" s="13"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
+      <c r="F35" s="13"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="L35" s="13"/>
       <c r="M35" s="8"/>
       <c r="N35" s="8"/>
       <c r="O35" s="15"/>
@@ -2705,7 +2708,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="36" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" style="32" customWidth="1"/>
     <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -2714,71 +2717,71 @@
   <sheetData>
     <row r="1" spans="1:18" ht="3" customHeight="1"/>
     <row r="2" spans="1:18" ht="15" customHeight="1">
-      <c r="A2" s="36">
+      <c r="A2" s="32">
         <f>A1+1</f>
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1">
-      <c r="A3" s="36">
+      <c r="A3" s="32">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1">
-      <c r="A4" s="36">
-        <f t="shared" ref="A4:A36" si="0">A3+1</f>
+      <c r="A4" s="32">
+        <f t="shared" ref="A4:A35" si="0">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1">
-      <c r="A5" s="36">
+      <c r="A5" s="32">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="36">
+      <c r="A6" s="32">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -2796,7 +2799,7 @@
       </c>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="36">
+      <c r="A7" s="32">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -2814,7 +2817,7 @@
       </c>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="36">
+      <c r="A8" s="32">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -2832,7 +2835,7 @@
       </c>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="36">
+      <c r="A9" s="32">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -2850,7 +2853,7 @@
       </c>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="36">
+      <c r="A10" s="32">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -2868,7 +2871,7 @@
       </c>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="36">
+      <c r="A11" s="32">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -2886,7 +2889,7 @@
       </c>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="36">
+      <c r="A12" s="32">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -2904,7 +2907,7 @@
       </c>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="36">
+      <c r="A13" s="32">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -2922,7 +2925,7 @@
       </c>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="36">
+      <c r="A14" s="32">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -2940,7 +2943,7 @@
       </c>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="36">
+      <c r="A15" s="32">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -2958,7 +2961,7 @@
       </c>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="36">
+      <c r="A16" s="32">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -2976,7 +2979,7 @@
       </c>
     </row>
     <row r="17" spans="1:24">
-      <c r="A17" s="36">
+      <c r="A17" s="32">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -2990,95 +2993,95 @@
       <c r="M18" s="26"/>
     </row>
     <row r="19" spans="1:24">
-      <c r="A19" s="36">
+      <c r="A19" s="32">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="P19" s="34" t="s">
+      <c r="P19" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="Q19" s="35"/>
-      <c r="R19" s="35"/>
-      <c r="S19" s="35"/>
-      <c r="T19" s="35"/>
-      <c r="U19" s="35"/>
-      <c r="V19" s="35"/>
-      <c r="W19" s="35"/>
-      <c r="X19" s="35"/>
+      <c r="Q19" s="43"/>
+      <c r="R19" s="43"/>
+      <c r="S19" s="43"/>
+      <c r="T19" s="43"/>
+      <c r="U19" s="43"/>
+      <c r="V19" s="43"/>
+      <c r="W19" s="43"/>
+      <c r="X19" s="43"/>
     </row>
     <row r="20" spans="1:24">
-      <c r="A20" s="36">
+      <c r="A20" s="32">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="P20" s="35"/>
-      <c r="Q20" s="35"/>
-      <c r="R20" s="35"/>
-      <c r="S20" s="35"/>
-      <c r="T20" s="35"/>
-      <c r="U20" s="35"/>
-      <c r="V20" s="35"/>
-      <c r="W20" s="35"/>
-      <c r="X20" s="35"/>
+      <c r="P20" s="43"/>
+      <c r="Q20" s="43"/>
+      <c r="R20" s="43"/>
+      <c r="S20" s="43"/>
+      <c r="T20" s="43"/>
+      <c r="U20" s="43"/>
+      <c r="V20" s="43"/>
+      <c r="W20" s="43"/>
+      <c r="X20" s="43"/>
     </row>
     <row r="21" spans="1:24">
-      <c r="A21" s="36">
+      <c r="A21" s="32">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="P21" s="34" t="s">
+      <c r="P21" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="Q21" s="35"/>
-      <c r="R21" s="35"/>
-      <c r="S21" s="35"/>
-      <c r="T21" s="35"/>
-      <c r="U21" s="35"/>
-      <c r="V21" s="35"/>
-      <c r="W21" s="35"/>
-      <c r="X21" s="35"/>
+      <c r="Q21" s="43"/>
+      <c r="R21" s="43"/>
+      <c r="S21" s="43"/>
+      <c r="T21" s="43"/>
+      <c r="U21" s="43"/>
+      <c r="V21" s="43"/>
+      <c r="W21" s="43"/>
+      <c r="X21" s="43"/>
     </row>
     <row r="22" spans="1:24">
-      <c r="A22" s="36">
+      <c r="A22" s="32">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="P22" s="35"/>
-      <c r="Q22" s="35"/>
-      <c r="R22" s="35"/>
-      <c r="S22" s="35"/>
-      <c r="T22" s="35"/>
-      <c r="U22" s="35"/>
-      <c r="V22" s="35"/>
-      <c r="W22" s="35"/>
-      <c r="X22" s="35"/>
+      <c r="P22" s="43"/>
+      <c r="Q22" s="43"/>
+      <c r="R22" s="43"/>
+      <c r="S22" s="43"/>
+      <c r="T22" s="43"/>
+      <c r="U22" s="43"/>
+      <c r="V22" s="43"/>
+      <c r="W22" s="43"/>
+      <c r="X22" s="43"/>
     </row>
     <row r="23" spans="1:24">
-      <c r="A23" s="36">
+      <c r="A23" s="32">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:24">
-      <c r="A24" s="36">
+      <c r="A24" s="32">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="P24" s="37" t="s">
+      <c r="P24" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="Q24" s="37"/>
-      <c r="R24" s="37"/>
-      <c r="S24" s="37"/>
-      <c r="T24" s="37"/>
-      <c r="U24" s="37"/>
-      <c r="V24" s="37"/>
-      <c r="W24" s="38">
+      <c r="Q24" s="33"/>
+      <c r="R24" s="33"/>
+      <c r="S24" s="33"/>
+      <c r="T24" s="33"/>
+      <c r="U24" s="33"/>
+      <c r="V24" s="33"/>
+      <c r="W24" s="34">
         <v>0.24097222222222223</v>
       </c>
     </row>
     <row r="25" spans="1:24">
-      <c r="A25" s="36">
+      <c r="A25" s="32">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -3096,7 +3099,7 @@
       </c>
     </row>
     <row r="26" spans="1:24">
-      <c r="A26" s="36">
+      <c r="A26" s="32">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -3114,7 +3117,7 @@
       </c>
     </row>
     <row r="27" spans="1:24">
-      <c r="A27" s="36">
+      <c r="A27" s="32">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -3132,7 +3135,7 @@
       </c>
     </row>
     <row r="28" spans="1:24">
-      <c r="A28" s="36">
+      <c r="A28" s="32">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -3150,7 +3153,7 @@
       </c>
     </row>
     <row r="29" spans="1:24">
-      <c r="A29" s="36">
+      <c r="A29" s="32">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -3168,7 +3171,7 @@
       </c>
     </row>
     <row r="30" spans="1:24">
-      <c r="A30" s="36">
+      <c r="A30" s="32">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -3186,7 +3189,7 @@
       </c>
     </row>
     <row r="31" spans="1:24">
-      <c r="A31" s="36">
+      <c r="A31" s="32">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -3204,7 +3207,7 @@
       </c>
     </row>
     <row r="32" spans="1:24">
-      <c r="A32" s="36">
+      <c r="A32" s="32">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -3222,7 +3225,7 @@
       </c>
     </row>
     <row r="33" spans="1:23">
-      <c r="A33" s="36">
+      <c r="A33" s="32">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -3240,7 +3243,7 @@
       </c>
     </row>
     <row r="34" spans="1:23">
-      <c r="A34" s="36">
+      <c r="A34" s="32">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -3253,16 +3256,16 @@
       <c r="T34" s="28"/>
       <c r="U34" s="28"/>
       <c r="V34" s="28"/>
-      <c r="W34" s="42">
+      <c r="W34" s="38">
         <v>0.44930555555555557</v>
       </c>
     </row>
     <row r="35" spans="1:23">
-      <c r="A35" s="36">
+      <c r="A35" s="32">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="W35" s="40" t="s">
+      <c r="W35" s="36" t="s">
         <v>97</v>
       </c>
     </row>
@@ -3283,13 +3286,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="V39" sqref="V39"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="V55" sqref="V55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="36" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" style="32" customWidth="1"/>
     <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -3300,83 +3303,83 @@
   <sheetData>
     <row r="1" spans="1:27" ht="3" customHeight="1"/>
     <row r="2" spans="1:27" ht="15" customHeight="1">
-      <c r="A2" s="36">
+      <c r="A2" s="32">
         <f>A1+1</f>
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
     </row>
     <row r="3" spans="1:27" ht="15" customHeight="1">
-      <c r="A3" s="36">
+      <c r="A3" s="32">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1">
-      <c r="A4" s="36">
+      <c r="A4" s="32">
         <f t="shared" ref="A4:A38" si="0">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1">
-      <c r="A5" s="36">
+      <c r="A5" s="32">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
     </row>
     <row r="6" spans="1:27">
-      <c r="A6" s="36">
+      <c r="A6" s="32">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="K6" s="39" t="s">
+      <c r="K6" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="T6" s="39" t="s">
+      <c r="T6" s="35" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:27">
-      <c r="A7" s="36">
+      <c r="A7" s="32">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -3402,7 +3405,7 @@
       </c>
     </row>
     <row r="8" spans="1:27">
-      <c r="A8" s="36">
+      <c r="A8" s="32">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -3432,7 +3435,7 @@
       </c>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" s="36">
+      <c r="A9" s="32">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -3462,7 +3465,7 @@
       </c>
     </row>
     <row r="10" spans="1:27">
-      <c r="A10" s="36">
+      <c r="A10" s="32">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -3492,7 +3495,7 @@
       </c>
     </row>
     <row r="11" spans="1:27">
-      <c r="A11" s="36">
+      <c r="A11" s="32">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -3522,7 +3525,7 @@
       </c>
     </row>
     <row r="12" spans="1:27">
-      <c r="A12" s="36">
+      <c r="A12" s="32">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -3552,7 +3555,7 @@
       </c>
     </row>
     <row r="13" spans="1:27">
-      <c r="A13" s="36">
+      <c r="A13" s="32">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -3582,7 +3585,7 @@
       </c>
     </row>
     <row r="14" spans="1:27">
-      <c r="A14" s="36">
+      <c r="A14" s="32">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -3612,7 +3615,7 @@
       </c>
     </row>
     <row r="15" spans="1:27">
-      <c r="A15" s="36">
+      <c r="A15" s="32">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -3630,7 +3633,7 @@
       </c>
     </row>
     <row r="16" spans="1:27">
-      <c r="A16" s="36">
+      <c r="A16" s="32">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -3648,7 +3651,7 @@
       </c>
     </row>
     <row r="17" spans="1:32">
-      <c r="A17" s="36">
+      <c r="A17" s="32">
         <f>A15+1</f>
         <v>15</v>
       </c>
@@ -3666,7 +3669,7 @@
       </c>
     </row>
     <row r="18" spans="1:32">
-      <c r="A18" s="36">
+      <c r="A18" s="32">
         <f>A16+1</f>
         <v>16</v>
       </c>
@@ -3692,71 +3695,71 @@
       <c r="M19" s="26"/>
     </row>
     <row r="20" spans="1:32">
-      <c r="A20" s="36">
+      <c r="A20" s="32">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="P20" s="32" t="s">
+      <c r="P20" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="Q20" s="33"/>
-      <c r="R20" s="33"/>
-      <c r="S20" s="33"/>
-      <c r="T20" s="33"/>
-      <c r="U20" s="33"/>
-      <c r="V20" s="33"/>
-      <c r="W20" s="33"/>
-      <c r="X20" s="33"/>
+      <c r="Q20" s="41"/>
+      <c r="R20" s="41"/>
+      <c r="S20" s="41"/>
+      <c r="T20" s="41"/>
+      <c r="U20" s="41"/>
+      <c r="V20" s="41"/>
+      <c r="W20" s="41"/>
+      <c r="X20" s="41"/>
     </row>
     <row r="21" spans="1:32">
-      <c r="A21" s="36">
+      <c r="A21" s="32">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="P21" s="33"/>
-      <c r="Q21" s="33"/>
-      <c r="R21" s="33"/>
-      <c r="S21" s="33"/>
-      <c r="T21" s="33"/>
-      <c r="U21" s="33"/>
-      <c r="V21" s="33"/>
-      <c r="W21" s="33"/>
-      <c r="X21" s="33"/>
+      <c r="P21" s="41"/>
+      <c r="Q21" s="41"/>
+      <c r="R21" s="41"/>
+      <c r="S21" s="41"/>
+      <c r="T21" s="41"/>
+      <c r="U21" s="41"/>
+      <c r="V21" s="41"/>
+      <c r="W21" s="41"/>
+      <c r="X21" s="41"/>
     </row>
     <row r="22" spans="1:32">
-      <c r="A22" s="36">
+      <c r="A22" s="32">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="P22" s="34" t="s">
+      <c r="P22" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="Q22" s="35"/>
-      <c r="R22" s="35"/>
-      <c r="S22" s="35"/>
-      <c r="T22" s="35"/>
-      <c r="U22" s="35"/>
-      <c r="V22" s="35"/>
-      <c r="W22" s="35"/>
-      <c r="X22" s="35"/>
+      <c r="Q22" s="43"/>
+      <c r="R22" s="43"/>
+      <c r="S22" s="43"/>
+      <c r="T22" s="43"/>
+      <c r="U22" s="43"/>
+      <c r="V22" s="43"/>
+      <c r="W22" s="43"/>
+      <c r="X22" s="43"/>
     </row>
     <row r="23" spans="1:32">
-      <c r="A23" s="36">
+      <c r="A23" s="32">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="P23" s="35"/>
-      <c r="Q23" s="35"/>
-      <c r="R23" s="35"/>
-      <c r="S23" s="35"/>
-      <c r="T23" s="35"/>
-      <c r="U23" s="35"/>
-      <c r="V23" s="35"/>
-      <c r="W23" s="35"/>
-      <c r="X23" s="35"/>
+      <c r="P23" s="43"/>
+      <c r="Q23" s="43"/>
+      <c r="R23" s="43"/>
+      <c r="S23" s="43"/>
+      <c r="T23" s="43"/>
+      <c r="U23" s="43"/>
+      <c r="V23" s="43"/>
+      <c r="W23" s="43"/>
+      <c r="X23" s="43"/>
     </row>
     <row r="24" spans="1:32">
-      <c r="A24" s="36">
+      <c r="A24" s="32">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -3765,25 +3768,25 @@
       </c>
     </row>
     <row r="25" spans="1:32">
-      <c r="A25" s="36">
+      <c r="A25" s="32">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:32">
-      <c r="A26" s="36">
+      <c r="A26" s="32">
         <f>A23+1</f>
         <v>5</v>
       </c>
-      <c r="P26" s="39" t="s">
+      <c r="P26" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="Y26" s="39" t="s">
+      <c r="Y26" s="35" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:32">
-      <c r="A27" s="36">
+      <c r="A27" s="32">
         <f>A24+1</f>
         <v>6</v>
       </c>
@@ -3809,20 +3812,20 @@
       </c>
     </row>
     <row r="28" spans="1:32">
-      <c r="A28" s="36">
+      <c r="A28" s="32">
         <f>A25+1</f>
         <v>7</v>
       </c>
-      <c r="P28" s="37" t="s">
+      <c r="P28" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="Q28" s="37"/>
-      <c r="R28" s="37"/>
-      <c r="S28" s="37"/>
-      <c r="T28" s="37"/>
-      <c r="U28" s="37"/>
-      <c r="V28" s="37"/>
-      <c r="W28" s="38">
+      <c r="Q28" s="33"/>
+      <c r="R28" s="33"/>
+      <c r="S28" s="33"/>
+      <c r="T28" s="33"/>
+      <c r="U28" s="33"/>
+      <c r="V28" s="33"/>
+      <c r="W28" s="34">
         <v>0.24097222222222223</v>
       </c>
       <c r="Y28" s="26" t="s">
@@ -3839,7 +3842,7 @@
       </c>
     </row>
     <row r="29" spans="1:32">
-      <c r="A29" s="36">
+      <c r="A29" s="32">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -3869,7 +3872,7 @@
       </c>
     </row>
     <row r="30" spans="1:32">
-      <c r="A30" s="36">
+      <c r="A30" s="32">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -3899,7 +3902,7 @@
       </c>
     </row>
     <row r="31" spans="1:32">
-      <c r="A31" s="36">
+      <c r="A31" s="32">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -3929,7 +3932,7 @@
       </c>
     </row>
     <row r="32" spans="1:32">
-      <c r="A32" s="36">
+      <c r="A32" s="32">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -3959,7 +3962,7 @@
       </c>
     </row>
     <row r="33" spans="1:32">
-      <c r="A33" s="36">
+      <c r="A33" s="32">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -3989,7 +3992,7 @@
       </c>
     </row>
     <row r="34" spans="1:32">
-      <c r="A34" s="36">
+      <c r="A34" s="32">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -4019,7 +4022,7 @@
       </c>
     </row>
     <row r="35" spans="1:32">
-      <c r="A35" s="36">
+      <c r="A35" s="32">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -4037,7 +4040,7 @@
       </c>
     </row>
     <row r="36" spans="1:32">
-      <c r="A36" s="36">
+      <c r="A36" s="32">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -4055,7 +4058,7 @@
       </c>
     </row>
     <row r="37" spans="1:32">
-      <c r="A37" s="36">
+      <c r="A37" s="32">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -4073,7 +4076,7 @@
       </c>
     </row>
     <row r="38" spans="1:32">
-      <c r="A38" s="36">
+      <c r="A38" s="32">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -4096,119 +4099,119 @@
       <c r="M39" s="26"/>
     </row>
     <row r="40" spans="1:32">
-      <c r="A40" s="36">
+      <c r="A40" s="32">
         <f t="shared" ref="A40:A46" si="1">A39+1</f>
         <v>1</v>
       </c>
-      <c r="P40" s="32" t="s">
+      <c r="P40" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="Q40" s="33"/>
-      <c r="R40" s="33"/>
-      <c r="S40" s="33"/>
-      <c r="T40" s="33"/>
-      <c r="U40" s="33"/>
-      <c r="V40" s="33"/>
-      <c r="W40" s="33"/>
-      <c r="X40" s="33"/>
+      <c r="Q40" s="41"/>
+      <c r="R40" s="41"/>
+      <c r="S40" s="41"/>
+      <c r="T40" s="41"/>
+      <c r="U40" s="41"/>
+      <c r="V40" s="41"/>
+      <c r="W40" s="41"/>
+      <c r="X40" s="41"/>
     </row>
     <row r="41" spans="1:32">
-      <c r="A41" s="36">
+      <c r="A41" s="32">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="P41" s="33"/>
-      <c r="Q41" s="33"/>
-      <c r="R41" s="33"/>
-      <c r="S41" s="33"/>
-      <c r="T41" s="33"/>
-      <c r="U41" s="33"/>
-      <c r="V41" s="33"/>
-      <c r="W41" s="33"/>
-      <c r="X41" s="33"/>
+      <c r="P41" s="41"/>
+      <c r="Q41" s="41"/>
+      <c r="R41" s="41"/>
+      <c r="S41" s="41"/>
+      <c r="T41" s="41"/>
+      <c r="U41" s="41"/>
+      <c r="V41" s="41"/>
+      <c r="W41" s="41"/>
+      <c r="X41" s="41"/>
     </row>
     <row r="42" spans="1:32">
-      <c r="A42" s="36">
+      <c r="A42" s="32">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="P42" s="34" t="s">
+      <c r="P42" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="Q42" s="35"/>
-      <c r="R42" s="35"/>
-      <c r="S42" s="35"/>
-      <c r="T42" s="35"/>
-      <c r="U42" s="35"/>
-      <c r="V42" s="35"/>
-      <c r="W42" s="35"/>
-      <c r="X42" s="35"/>
+      <c r="Q42" s="43"/>
+      <c r="R42" s="43"/>
+      <c r="S42" s="43"/>
+      <c r="T42" s="43"/>
+      <c r="U42" s="43"/>
+      <c r="V42" s="43"/>
+      <c r="W42" s="43"/>
+      <c r="X42" s="43"/>
     </row>
     <row r="43" spans="1:32">
-      <c r="A43" s="36">
+      <c r="A43" s="32">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="P43" s="35"/>
-      <c r="Q43" s="35"/>
-      <c r="R43" s="35"/>
-      <c r="S43" s="35"/>
-      <c r="T43" s="35"/>
-      <c r="U43" s="35"/>
-      <c r="V43" s="35"/>
-      <c r="W43" s="35"/>
-      <c r="X43" s="35"/>
+      <c r="P43" s="43"/>
+      <c r="Q43" s="43"/>
+      <c r="R43" s="43"/>
+      <c r="S43" s="43"/>
+      <c r="T43" s="43"/>
+      <c r="U43" s="43"/>
+      <c r="V43" s="43"/>
+      <c r="W43" s="43"/>
+      <c r="X43" s="43"/>
     </row>
     <row r="44" spans="1:32">
-      <c r="A44" s="36">
+      <c r="A44" s="32">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:32">
-      <c r="A45" s="36">
+      <c r="A45" s="32">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="P45" s="39" t="s">
+      <c r="P45" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="Y45" s="39" t="s">
+      <c r="Y45" s="35" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:32">
-      <c r="A46" s="36">
+      <c r="A46" s="32">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="P46" s="37" t="s">
+      <c r="P46" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="Q46" s="37"/>
-      <c r="R46" s="37"/>
-      <c r="S46" s="37"/>
-      <c r="T46" s="37"/>
-      <c r="U46" s="37"/>
-      <c r="V46" s="37"/>
-      <c r="W46" s="38">
+      <c r="Q46" s="33"/>
+      <c r="R46" s="33"/>
+      <c r="S46" s="33"/>
+      <c r="T46" s="33"/>
+      <c r="U46" s="33"/>
+      <c r="V46" s="33"/>
+      <c r="W46" s="34">
         <v>0.24097222222222223</v>
       </c>
-      <c r="Y46" s="37" t="s">
+      <c r="Y46" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="Z46" s="37"/>
-      <c r="AA46" s="37"/>
-      <c r="AB46" s="37"/>
-      <c r="AC46" s="37"/>
-      <c r="AD46" s="37"/>
-      <c r="AE46" s="37"/>
-      <c r="AF46" s="38">
+      <c r="Z46" s="33"/>
+      <c r="AA46" s="33"/>
+      <c r="AB46" s="33"/>
+      <c r="AC46" s="33"/>
+      <c r="AD46" s="33"/>
+      <c r="AE46" s="33"/>
+      <c r="AF46" s="34">
         <v>0.24097222222222223</v>
       </c>
     </row>
     <row r="47" spans="1:32">
-      <c r="A47" s="36">
+      <c r="A47" s="32">
         <f>A44+1</f>
         <v>6</v>
       </c>
@@ -4233,12 +4236,12 @@
       <c r="AC47" s="29"/>
       <c r="AD47" s="29"/>
       <c r="AE47" s="29"/>
-      <c r="AF47" s="41">
+      <c r="AF47" s="37">
         <v>0.19305555555555554</v>
       </c>
     </row>
     <row r="48" spans="1:32">
-      <c r="A48" s="36">
+      <c r="A48" s="32">
         <f t="shared" ref="A48:A57" si="2">A47+1</f>
         <v>7</v>
       </c>
@@ -4263,12 +4266,12 @@
       <c r="AC48" s="29"/>
       <c r="AD48" s="29"/>
       <c r="AE48" s="29"/>
-      <c r="AF48" s="41">
+      <c r="AF48" s="37">
         <v>0.34791666666666665</v>
       </c>
     </row>
     <row r="49" spans="1:32">
-      <c r="A49" s="36">
+      <c r="A49" s="32">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
@@ -4293,12 +4296,12 @@
       <c r="AC49" s="29"/>
       <c r="AD49" s="29"/>
       <c r="AE49" s="29"/>
-      <c r="AF49" s="41">
+      <c r="AF49" s="37">
         <v>0.18611111111111112</v>
       </c>
     </row>
     <row r="50" spans="1:32">
-      <c r="A50" s="36">
+      <c r="A50" s="32">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
@@ -4323,12 +4326,12 @@
       <c r="AC50" s="29"/>
       <c r="AD50" s="29"/>
       <c r="AE50" s="29"/>
-      <c r="AF50" s="41">
+      <c r="AF50" s="37">
         <v>0.32708333333333334</v>
       </c>
     </row>
     <row r="51" spans="1:32">
-      <c r="A51" s="36">
+      <c r="A51" s="32">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
@@ -4353,12 +4356,12 @@
       <c r="AC51" s="29"/>
       <c r="AD51" s="29"/>
       <c r="AE51" s="29"/>
-      <c r="AF51" s="41">
+      <c r="AF51" s="37">
         <v>0.20416666666666669</v>
       </c>
     </row>
     <row r="52" spans="1:32">
-      <c r="A52" s="36">
+      <c r="A52" s="32">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
@@ -4383,12 +4386,12 @@
       <c r="AC52" s="29"/>
       <c r="AD52" s="29"/>
       <c r="AE52" s="29"/>
-      <c r="AF52" s="41">
+      <c r="AF52" s="37">
         <v>7.6388888888888895E-2</v>
       </c>
     </row>
     <row r="53" spans="1:32">
-      <c r="A53" s="36">
+      <c r="A53" s="32">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
@@ -4414,7 +4417,7 @@
       <c r="AF53" s="8"/>
     </row>
     <row r="54" spans="1:32">
-      <c r="A54" s="36">
+      <c r="A54" s="32">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
@@ -4440,7 +4443,7 @@
       <c r="AF54" s="8"/>
     </row>
     <row r="55" spans="1:32">
-      <c r="A55" s="36">
+      <c r="A55" s="32">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
@@ -4466,7 +4469,7 @@
       <c r="AF55" s="8"/>
     </row>
     <row r="56" spans="1:32">
-      <c r="A56" s="36">
+      <c r="A56" s="32">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
@@ -4492,7 +4495,7 @@
       <c r="AF56" s="6"/>
     </row>
     <row r="57" spans="1:32">
-      <c r="A57" s="36">
+      <c r="A57" s="32">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
@@ -4503,10 +4506,10 @@
       <c r="T57" s="17"/>
       <c r="U57" s="17"/>
       <c r="V57" s="17"/>
-      <c r="W57" s="40" t="s">
+      <c r="W57" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="AF57" s="43" t="s">
+      <c r="AF57" s="39" t="s">
         <v>97</v>
       </c>
     </row>
@@ -4516,119 +4519,119 @@
       <c r="M58" s="26"/>
     </row>
     <row r="59" spans="1:32">
-      <c r="A59" s="36">
+      <c r="A59" s="32">
         <f t="shared" ref="A59:A65" si="3">A58+1</f>
         <v>1</v>
       </c>
-      <c r="P59" s="32" t="s">
+      <c r="P59" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="Q59" s="33"/>
-      <c r="R59" s="33"/>
-      <c r="S59" s="33"/>
-      <c r="T59" s="33"/>
-      <c r="U59" s="33"/>
-      <c r="V59" s="33"/>
-      <c r="W59" s="33"/>
-      <c r="X59" s="33"/>
+      <c r="Q59" s="41"/>
+      <c r="R59" s="41"/>
+      <c r="S59" s="41"/>
+      <c r="T59" s="41"/>
+      <c r="U59" s="41"/>
+      <c r="V59" s="41"/>
+      <c r="W59" s="41"/>
+      <c r="X59" s="41"/>
     </row>
     <row r="60" spans="1:32">
-      <c r="A60" s="36">
+      <c r="A60" s="32">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="P60" s="33"/>
-      <c r="Q60" s="33"/>
-      <c r="R60" s="33"/>
-      <c r="S60" s="33"/>
-      <c r="T60" s="33"/>
-      <c r="U60" s="33"/>
-      <c r="V60" s="33"/>
-      <c r="W60" s="33"/>
-      <c r="X60" s="33"/>
+      <c r="P60" s="41"/>
+      <c r="Q60" s="41"/>
+      <c r="R60" s="41"/>
+      <c r="S60" s="41"/>
+      <c r="T60" s="41"/>
+      <c r="U60" s="41"/>
+      <c r="V60" s="41"/>
+      <c r="W60" s="41"/>
+      <c r="X60" s="41"/>
     </row>
     <row r="61" spans="1:32">
-      <c r="A61" s="36">
+      <c r="A61" s="32">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="P61" s="34" t="s">
+      <c r="P61" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="Q61" s="35"/>
-      <c r="R61" s="35"/>
-      <c r="S61" s="35"/>
-      <c r="T61" s="35"/>
-      <c r="U61" s="35"/>
-      <c r="V61" s="35"/>
-      <c r="W61" s="35"/>
-      <c r="X61" s="35"/>
+      <c r="Q61" s="43"/>
+      <c r="R61" s="43"/>
+      <c r="S61" s="43"/>
+      <c r="T61" s="43"/>
+      <c r="U61" s="43"/>
+      <c r="V61" s="43"/>
+      <c r="W61" s="43"/>
+      <c r="X61" s="43"/>
     </row>
     <row r="62" spans="1:32">
-      <c r="A62" s="36">
+      <c r="A62" s="32">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="P62" s="35"/>
-      <c r="Q62" s="35"/>
-      <c r="R62" s="35"/>
-      <c r="S62" s="35"/>
-      <c r="T62" s="35"/>
-      <c r="U62" s="35"/>
-      <c r="V62" s="35"/>
-      <c r="W62" s="35"/>
-      <c r="X62" s="35"/>
+      <c r="P62" s="43"/>
+      <c r="Q62" s="43"/>
+      <c r="R62" s="43"/>
+      <c r="S62" s="43"/>
+      <c r="T62" s="43"/>
+      <c r="U62" s="43"/>
+      <c r="V62" s="43"/>
+      <c r="W62" s="43"/>
+      <c r="X62" s="43"/>
     </row>
     <row r="63" spans="1:32">
-      <c r="A63" s="36">
+      <c r="A63" s="32">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:32">
-      <c r="A64" s="36">
+      <c r="A64" s="32">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="P64" s="39" t="s">
+      <c r="P64" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="Y64" s="39" t="s">
+      <c r="Y64" s="35" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="65" spans="1:32">
-      <c r="A65" s="36">
+      <c r="A65" s="32">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="P65" s="37" t="s">
+      <c r="P65" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="Q65" s="37"/>
-      <c r="R65" s="37"/>
-      <c r="S65" s="37"/>
-      <c r="T65" s="37"/>
-      <c r="U65" s="37"/>
-      <c r="V65" s="37"/>
-      <c r="W65" s="38">
+      <c r="Q65" s="33"/>
+      <c r="R65" s="33"/>
+      <c r="S65" s="33"/>
+      <c r="T65" s="33"/>
+      <c r="U65" s="33"/>
+      <c r="V65" s="33"/>
+      <c r="W65" s="34">
         <v>0.24097222222222223</v>
       </c>
-      <c r="Y65" s="37" t="s">
+      <c r="Y65" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="Z65" s="37"/>
-      <c r="AA65" s="37"/>
-      <c r="AB65" s="37"/>
-      <c r="AC65" s="37"/>
-      <c r="AD65" s="37"/>
-      <c r="AE65" s="37"/>
-      <c r="AF65" s="38">
+      <c r="Z65" s="33"/>
+      <c r="AA65" s="33"/>
+      <c r="AB65" s="33"/>
+      <c r="AC65" s="33"/>
+      <c r="AD65" s="33"/>
+      <c r="AE65" s="33"/>
+      <c r="AF65" s="34">
         <v>0.24097222222222223</v>
       </c>
     </row>
     <row r="66" spans="1:32">
-      <c r="A66" s="36">
+      <c r="A66" s="32">
         <f>A63+1</f>
         <v>6</v>
       </c>
@@ -4653,12 +4656,12 @@
       <c r="AC66" s="29"/>
       <c r="AD66" s="29"/>
       <c r="AE66" s="29"/>
-      <c r="AF66" s="41">
+      <c r="AF66" s="37">
         <v>0.19305555555555554</v>
       </c>
     </row>
     <row r="67" spans="1:32">
-      <c r="A67" s="36">
+      <c r="A67" s="32">
         <f t="shared" ref="A67:A76" si="4">A66+1</f>
         <v>7</v>
       </c>
@@ -4683,12 +4686,12 @@
       <c r="AC67" s="29"/>
       <c r="AD67" s="29"/>
       <c r="AE67" s="29"/>
-      <c r="AF67" s="41">
+      <c r="AF67" s="37">
         <v>0.34791666666666665</v>
       </c>
     </row>
     <row r="68" spans="1:32">
-      <c r="A68" s="36">
+      <c r="A68" s="32">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
@@ -4713,12 +4716,12 @@
       <c r="AC68" s="29"/>
       <c r="AD68" s="29"/>
       <c r="AE68" s="29"/>
-      <c r="AF68" s="41">
+      <c r="AF68" s="37">
         <v>0.18611111111111112</v>
       </c>
     </row>
     <row r="69" spans="1:32">
-      <c r="A69" s="36">
+      <c r="A69" s="32">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
@@ -4743,12 +4746,12 @@
       <c r="AC69" s="29"/>
       <c r="AD69" s="29"/>
       <c r="AE69" s="29"/>
-      <c r="AF69" s="41">
+      <c r="AF69" s="37">
         <v>0.32708333333333334</v>
       </c>
     </row>
     <row r="70" spans="1:32">
-      <c r="A70" s="36">
+      <c r="A70" s="32">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
@@ -4773,12 +4776,12 @@
       <c r="AC70" s="29"/>
       <c r="AD70" s="29"/>
       <c r="AE70" s="29"/>
-      <c r="AF70" s="41">
+      <c r="AF70" s="37">
         <v>0.20416666666666669</v>
       </c>
     </row>
     <row r="71" spans="1:32">
-      <c r="A71" s="36">
+      <c r="A71" s="32">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
@@ -4803,12 +4806,12 @@
       <c r="AC71" s="29"/>
       <c r="AD71" s="29"/>
       <c r="AE71" s="29"/>
-      <c r="AF71" s="41">
+      <c r="AF71" s="37">
         <v>7.6388888888888895E-2</v>
       </c>
     </row>
     <row r="72" spans="1:32">
-      <c r="A72" s="36">
+      <c r="A72" s="32">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
@@ -4831,12 +4834,12 @@
       <c r="AC72" s="17"/>
       <c r="AD72" s="17"/>
       <c r="AE72" s="17"/>
-      <c r="AF72" s="40" t="s">
+      <c r="AF72" s="36" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="73" spans="1:32">
-      <c r="A73" s="36">
+      <c r="A73" s="32">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
@@ -4862,7 +4865,7 @@
       <c r="AF73" s="8"/>
     </row>
     <row r="74" spans="1:32">
-      <c r="A74" s="36">
+      <c r="A74" s="32">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
@@ -4888,7 +4891,7 @@
       <c r="AF74" s="8"/>
     </row>
     <row r="75" spans="1:32">
-      <c r="A75" s="36">
+      <c r="A75" s="32">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
@@ -4914,7 +4917,7 @@
       <c r="AF75" s="8"/>
     </row>
     <row r="76" spans="1:32">
-      <c r="A76" s="36">
+      <c r="A76" s="32">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
@@ -4925,7 +4928,7 @@
       <c r="T76" s="17"/>
       <c r="U76" s="17"/>
       <c r="V76" s="17"/>
-      <c r="W76" s="40" t="s">
+      <c r="W76" s="36" t="s">
         <v>97</v>
       </c>
     </row>

</xml_diff>